<commit_message>
Fri Nov  8 05:42:23 PM EST 2024
</commit_message>
<xml_diff>
--- a/SHAP/all_ozone_MB_shap.xlsx
+++ b/SHAP/all_ozone_MB_shap.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,122 +444,172 @@
           <t>shap</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rename</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SCFOCCp</t>
+          <t>pair_energy</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3.383324745841995e-07</v>
+        <v>3.066032814625092e-08</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$\left(\varepsilon_{pq}^{\text{MP2}}\right)$</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SCFOCCr4</t>
+          <t>occp</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8.873131587136632e-07</v>
+        <v>9.007481152173382e-08</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$\eta_{p}$</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SCFOCCs1</t>
+          <t>SCFOCCp</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9.704023177316094e-07</v>
+        <v>1.270633939540931e-07</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$\omega_{p}$</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SCFOCCs2</t>
+          <t>From_Same_Orbital</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9.828729123381715e-07</v>
+        <v>1.593924541623799e-07</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$\mathbf{b}$</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SCFFs3</t>
+          <t>occs2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9.857750396926709e-07</v>
+        <v>4.628921353146668e-07</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$(\eta_{s})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SCFOCCr3</t>
+          <t>SCFOCCs2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.034704488832886e-06</v>
+        <v>4.678064769433282e-07</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SCFOCCq</t>
+          <t>SCFOCCr3</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.067280305984442e-06</v>
+        <v>5.008621675651648e-07</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>hss1</t>
+          <t>SCFOCCs4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.067498616228606e-06</v>
+        <v>5.464256855049324e-07</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SCFOCCr1</t>
+          <t>SCFOCCr4</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.083706086938046e-06</v>
+        <v>5.831445850811643e-07</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -572,137 +622,192 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.120897089230763e-06</v>
+        <v>6.200483453274433e-07</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SCFOCCs4</t>
+          <t>SCFOCCr1</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1.43514282982455e-06</v>
+        <v>6.391552350343834e-07</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SCFOCCr2</t>
+          <t>SCFOCCs1</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1.49787499364351e-06</v>
+        <v>6.519000493303171e-07</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>occs1</t>
+          <t>SCFOCCq</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.532517184290726e-06</v>
+        <v>7.350618166646848e-07</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$\omega_{p}$</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>From_Same_Orbital</t>
+          <t>SCFFr2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1.844200371727157e-06</v>
+        <v>8.108092935484019e-07</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>hqq</t>
+          <t>SCFOCCr2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.958414665805541e-06</v>
+        <v>8.177592265648257e-07</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>eijab_3</t>
+          <t>SCFFr4</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.106162080807235e-06</v>
+        <v>1.069411449390139e-06</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$(F_{r}^{\text{SCF}})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SCFFr2</t>
+          <t>Fs2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.208830496436244e-06</v>
+        <v>1.395047250350745e-06</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$(F_{s})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Fs1</t>
+          <t>hqq</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.379649336766034e-06</v>
+        <v>1.948560491410678e-06</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$h_{qq}$</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SCFFs1</t>
+          <t>occs1</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.477390928995477e-06</v>
+        <v>2.783610736661349e-06</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$(\eta_{s})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>occp</t>
+          <t>hss4</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.980909665399226e-06</v>
+        <v>4.309347523130225e-06</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$(h_{ss})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -715,358 +820,498 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.651222311988656e-06</v>
+        <v>4.782354666913964e-06</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>$(h_{ss})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>hss4</t>
+          <t>hrr4</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.845223432854288e-06</v>
+        <v>5.98431378628151e-06</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>$(h_{rr})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>occr3</t>
+          <t>Fr3</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5.67520677131016e-06</v>
+        <v>9.005470993626747e-06</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>$(F_{r})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fs3</t>
+          <t>SCFFr3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6.19739469852633e-06</v>
+        <v>1.133333531881307e-05</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>occq</t>
+          <t>hrr2</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>7.030454224122697e-06</v>
+        <v>1.151941430186525e-05</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>$(h_{rr})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>occs3</t>
+          <t>SCFFs3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>7.428702796870561e-06</v>
+        <v>1.446614255483271e-05</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>$(F_{s}^{\text{SCF}})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SCFFr4</t>
+          <t>occs4</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>7.489180643692653e-06</v>
+        <v>1.621568835734885e-05</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>$(\eta_{s})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fs4</t>
+          <t>SCFFr1</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>8.761556775137066e-06</v>
+        <v>1.633159600448834e-05</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>occr4</t>
+          <t>Fr4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.749035551279383e-06</v>
+        <v>1.634412636579059e-05</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>$(F_{r})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>hrr3</t>
+          <t>occs3</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.24171677902743e-05</v>
+        <v>1.656437647339937e-05</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>$(\eta_{s})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SCFFp</t>
+          <t>hrr3</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.395885346038223e-05</v>
+        <v>1.809523655504705e-05</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>$(h_{rr})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>occs4</t>
+          <t>hrr1</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1.410845670911772e-05</v>
+        <v>1.896106418495491e-05</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>$(h_{rr})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Fs2</t>
+          <t>eijab_3</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.43457098344579e-05</v>
+        <v>1.989628732556284e-05</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>$(e^{rs}_{pq})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SCFFs4</t>
+          <t>Fr2</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1.438530236877726e-05</v>
+        <v>2.27742806884989e-05</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>$(F_{r})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>hss2</t>
+          <t>occr3</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.495222436128716e-05</v>
+        <v>2.287255070539599e-05</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>$(\eta_{r})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>hpp</t>
+          <t>Fs3</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1.527628759744439e-05</v>
+        <v>2.693023691802636e-05</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>$(F_{s})_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SCFFr3</t>
+          <t>eijab_4</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1.633993775406982e-05</v>
+        <v>2.793296040015019e-05</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>$(e^{rs}_{pq})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>hrr1</t>
+          <t>occr4</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.649385930228414e-05</v>
+        <v>2.912423636206734e-05</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>$(\eta_{r})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>hrr4</t>
+          <t>SCFFs4</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.861728169867345e-05</v>
+        <v>2.98289304025045e-05</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>$(F_{s}^{\text{SCF}})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fr3</t>
+          <t>hss1</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.91854634381263e-05</v>
+        <v>3.099170070176877e-05</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>$(h_{ss})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fr4</t>
+          <t>eijab_2</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2.030280534246464e-05</v>
+        <v>3.276834448683038e-05</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>$(e^{rs}_{pq})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Fr1</t>
+          <t>screen2_4</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2.931327460063032e-05</v>
+        <v>3.661295765833431e-05</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>$(\langle qq \vert \vert ss \rangle)_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SCFFr1</t>
+          <t>screenvirt_2</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.225415246436914e-05</v>
+        <v>3.78460080171781e-05</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>$(\langle ss \vert \vert rr \rangle)_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>screenvirt_4</t>
+          <t>Fr1</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.257160843500116e-05</v>
+        <v>3.859239089305153e-05</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>$(F_{r})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>eijab_2</t>
+          <t>eijab_1</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.276200713748728e-05</v>
+        <v>3.889256167491719e-05</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>$(e^{rs}_{pq})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>screenvirt_3</t>
+          <t>screenvirt_1</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.331704214826704e-05</v>
+        <v>3.905361518297251e-05</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>$(\langle ss \vert \vert rr \rangle)_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SCFFs2</t>
+          <t>occr2</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3.475344008038753e-05</v>
+        <v>4.020503578892763e-05</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>$(\eta_{r})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>screen1_2</t>
+          <t>occr1</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.548881534674982e-05</v>
+        <v>4.265310876794375e-05</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>$(\eta_{r})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1079,267 +1324,372 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.672106481604187e-05</v>
+        <v>4.472042494480772e-05</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>$F_{q}^{\text{SCF}}$</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>occr1</t>
+          <t>screen2_3</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.714454028112203e-05</v>
+        <v>4.517908053822079e-05</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>$(\langle qq \vert \vert ss \rangle)_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>screen1_3</t>
+          <t>Fp</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.845068303571862e-05</v>
+        <v>4.691652598230687e-05</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>$F_{p}$</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>occr2</t>
+          <t>Fs4</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.979432040070973e-05</v>
+        <v>5.324781947464344e-05</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>$(F_{s})_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>screenvirt_1</t>
+          <t>Fq</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4.442896079235047e-05</v>
+        <v>5.396310224662725e-05</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>$F_{q}$</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>coulomb</t>
+          <t>screen1_1</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4.655211859962944e-05</v>
+        <v>5.940879602786336e-05</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>$(\langle pp \vert \vert rr \rangle)_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>screen1_4</t>
+          <t>screen1_3</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5.571066903451575e-05</v>
+        <v>6.253773474039816e-05</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>$(\langle pp \vert \vert rr \rangle)_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>eijab_1</t>
+          <t>screenvirt_4</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>5.851115719717422e-05</v>
+        <v>6.732142213003006e-05</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>$(\langle ss \vert \vert rr \rangle)_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>screen2_2</t>
+          <t>screenvirt_3</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6.3406259596269e-05</v>
+        <v>7.208968252806431e-05</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>$(\langle ss \vert \vert rr \rangle)_{3}$</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>eijab_4</t>
+          <t>screen2_2</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>6.618027857216101e-05</v>
+        <v>7.35040271998253e-05</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>$(\langle qq \vert \vert ss \rangle)_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>screen2_1</t>
+          <t>screen1_2</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>7.537475996174948e-05</v>
+        <v>7.824272819801549e-05</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>$(\langle pp \vert \vert rr \rangle)_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>occs2</t>
+          <t>occq</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>8.959725207211664e-05</v>
+        <v>9.934645994097476e-05</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>$\eta_{q}$</t>
+        </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>hrr2</t>
+          <t>screen1_4</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>9.819208892460272e-05</v>
+        <v>0.0001148897168160615</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>$(\langle pp \vert \vert rr \rangle)_{4}$</t>
+        </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Fp</t>
+          <t>hpp</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.0001006899246613552</v>
+        <v>0.0001177320874143567</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>$h_{pp}$</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Fq</t>
+          <t>hss2</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.0001232189875433687</v>
+        <v>0.0001180824240041617</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>$(h_{ss})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Fr2</t>
+          <t>screen2_1</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.0001234222732746901</v>
+        <v>0.0001258499164456318</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>$(\langle qq \vert \vert ss \rangle)_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>screen2_3</t>
+          <t>SCFFp</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.0001259509578279438</v>
+        <v>0.0001755466996723631</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>$F_{p}^{\text{SCF}}$</t>
+        </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>screen2_4</t>
+          <t>Fs1</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.0001337095060248998</v>
+        <v>0.0001776322197255775</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>$(F_{s})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>pair_energy</t>
+          <t>SCFFs2</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.0001467576739154254</v>
+        <v>0.0001792907481552214</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>$(F_{s}^{\text{SCF}})_{2}$</t>
+        </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>screen1_1</t>
+          <t>SCFFs1</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.0001875505370739348</v>
+        <v>0.0002830631350236944</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>$(F_{s}^{\text{SCF}})_{1}$</t>
+        </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>screenvirt_2</t>
+          <t>coulomb</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.0002224156382649557</v>
+        <v>0.0003168259644355218</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>$\langle pp \vert \vert qq \rangle$</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>